<commit_message>
more graphs for inceptions score. steph is awesome! seems like its working
</commit_message>
<xml_diff>
--- a/results/inception_score.xlsx
+++ b/results/inception_score.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\cs231n_final\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dealmaker/projects/cs231n_final/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37EFFF20-C77B-47B1-A39B-DB02BA18E28B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6659EDC-1FC8-1247-9F10-1BCB4F641837}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="9204"/>
+    <workbookView xWindow="24100" yWindow="7860" windowWidth="40060" windowHeight="28960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inception_score" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>epoch_500</t>
   </si>
@@ -108,11 +108,32 @@
   <si>
     <t>elephant_transfer</t>
   </si>
+  <si>
+    <t>Gen updates</t>
+  </si>
+  <si>
+    <t>Inception Score</t>
+  </si>
+  <si>
+    <t>Fix epochs at 100</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>Fix at 300 Epochs</t>
+  </si>
+  <si>
+    <t>Gen Updates</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -590,8 +611,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2809,7 +2831,752 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Inception Score vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Gen Updates Elephants @ 300 epochs</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>inception_score!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inception Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>inception_score!$R$2:$R$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>inception_score!$S$2:$S$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.7334550000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3917164999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1004917999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4224-8644-9F8B-D81E0D69407C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1078927903"/>
+        <c:axId val="1078876847"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1078927903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1078876847"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1078876847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1078927903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Inception Score vs Gen Updates Elephants @ 100</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> epochs</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>inception_score!$N$2:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>inception_score!$O$2:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4810726999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8092031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4838214999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4817107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CCF8-CF46-B91C-135A5AF05E92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1189085183"/>
+        <c:axId val="1211634047"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1189085183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1211634047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1211634047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1189085183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3352,20 +4119,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1562100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>78740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>17780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3385,6 +5184,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{755A501A-C88C-F345-BFD5-B55E47BA91B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F466C0D9-D3A2-AC48-9778-85475C295806}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3689,20 +5560,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="87.6640625" customWidth="1"/>
-    <col min="8" max="9" width="11.88671875" customWidth="1"/>
+    <col min="8" max="9" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3733,8 +5606,26 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3762,32 +5653,83 @@
       <c r="I2">
         <v>2.6257454999999998</v>
       </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2.4810726999999999</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>2.7334550000000002</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
         <v>2.9914073999999999</v>
       </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>1.8092031</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>2.3917164999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4">
         <v>2.6013519999999999</v>
       </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="O4">
+        <v>1.4838214999999999</v>
+      </c>
+      <c r="R4">
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <v>2.1004917999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5">
         <v>2.4076675999999999</v>
       </c>
+      <c r="N5">
+        <v>20</v>
+      </c>
+      <c r="O5">
+        <v>1.4817107</v>
+      </c>
+      <c r="R5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -3798,15 +5740,24 @@
         <v>2.4545138</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7">
         <v>1.3314212999999999</v>
       </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>1.3314212999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -3819,16 +5770,28 @@
       <c r="F8">
         <v>4.0247780000000004</v>
       </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>2.143192</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9">
         <v>1.3647548</v>
       </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <v>1.3647548</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3841,8 +5804,14 @@
       <c r="F10">
         <v>2.6882066999999998</v>
       </c>
+      <c r="N10">
+        <v>40</v>
+      </c>
+      <c r="O10">
+        <v>1.3314212999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3850,7 +5819,7 @@
         <v>1.4817107</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3864,7 +5833,7 @@
         <v>3.2431958000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3875,7 +5844,7 @@
         <v>2.1004917999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -3883,7 +5852,7 @@
         <v>3.3723244999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3891,7 +5860,7 @@
         <v>2.5982751999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3899,7 +5868,7 @@
         <v>2.9396111999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -3907,7 +5876,7 @@
         <v>2.9009490000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3915,7 +5884,7 @@
         <v>2.7313013000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -3923,7 +5892,7 @@
         <v>3.5382639999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3933,6 +5902,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>